<commit_message>
working table counting rows
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danijeljw/Projects/FinReportBuilderCLI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220A880F-14A2-F944-A77D-10B9FB9D57E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A82EA3-B228-0144-B3C3-C36399798658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="1060" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{C0488145-81C1-A245-B336-D6EE4E12EADE}"/>
+    <workbookView xWindow="40700" yWindow="1080" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{C0488145-81C1-A245-B336-D6EE4E12EADE}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="1" r:id="rId1"/>
     <sheet name="Expenditure" sheetId="2" r:id="rId2"/>
+    <sheet name="CurrentAssets" sheetId="3" r:id="rId3"/>
+    <sheet name="NonCurrentAssets" sheetId="4" r:id="rId4"/>
+    <sheet name="CurrentLiabilities" sheetId="5" r:id="rId5"/>
+    <sheet name="NonCurrentLiabilities" sheetId="6" r:id="rId6"/>
+    <sheet name="Equity" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Note</t>
   </si>
@@ -64,6 +69,45 @@
   </si>
   <si>
     <t>Depreciation and New Asset Write Off</t>
+  </si>
+  <si>
+    <t>EQUITY</t>
+  </si>
+  <si>
+    <t>NON_CURRENT_LIABILITIES</t>
+  </si>
+  <si>
+    <t>CURRENT_LIABILITIES</t>
+  </si>
+  <si>
+    <t>NON_CURRENT_ASSETS</t>
+  </si>
+  <si>
+    <t>CURRENT_ASSETS</t>
+  </si>
+  <si>
+    <t>Trade and other receivables</t>
+  </si>
+  <si>
+    <t>Cash and cash equivalents</t>
+  </si>
+  <si>
+    <t>Property, plant and equipment</t>
+  </si>
+  <si>
+    <t>Intangible assets</t>
+  </si>
+  <si>
+    <t>Trade and Other Payables</t>
+  </si>
+  <si>
+    <t>Provision for Income Tax</t>
+  </si>
+  <si>
+    <t>Issued Capital</t>
+  </si>
+  <si>
+    <t>Reserves</t>
   </si>
 </sst>
 </file>
@@ -110,10 +154,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -431,12 +476,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA38823-0292-6644-A491-9C7A5884C41E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -446,10 +493,10 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="3">
         <v>2021</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="3">
         <v>2020</v>
       </c>
     </row>
@@ -457,10 +504,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>511376</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>545765</v>
       </c>
     </row>
@@ -473,14 +520,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC16966-3B3C-254F-BB2D-E9831DF66171}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -491,10 +538,10 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="3">
         <v>2021</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="3">
         <v>2020</v>
       </c>
     </row>
@@ -502,10 +549,10 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>-3250</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>-4614</v>
       </c>
     </row>
@@ -513,10 +560,10 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>-1358</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>-2340</v>
       </c>
     </row>
@@ -524,10 +571,10 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>-28880</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>-21750</v>
       </c>
     </row>
@@ -535,10 +582,10 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>-25576</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>-39644</v>
       </c>
     </row>
@@ -546,15 +593,227 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>-46474</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>-70049</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I9" s="2"/>
+      <c r="I9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166F594D-BC78-8144-A8D3-8BB1AF0D82A8}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34660CA8-F6EE-354F-A09C-EB1BD7F745BA}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3FB75A-DFF3-CB45-A965-E4F722630F8D}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DC8489-4E2C-0645-90D2-D38E8C166474}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02483EF2-613A-044D-ADCB-854E99DBC77E}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>2021</v>
+      </c>
+      <c r="D1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test ready to deploy to blazor
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danijeljw/Projects/FinReportBuilderCLI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A82EA3-B228-0144-B3C3-C36399798658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2934494F-EC0B-CD47-AA3F-A428626F63B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40700" yWindow="1080" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{C0488145-81C1-A245-B336-D6EE4E12EADE}"/>
+    <workbookView xWindow="43460" yWindow="2840" windowWidth="28040" windowHeight="17440" firstSheet="5" activeTab="12" xr2:uid="{C0488145-81C1-A245-B336-D6EE4E12EADE}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,12 @@
     <sheet name="CurrentLiabilities" sheetId="5" r:id="rId5"/>
     <sheet name="NonCurrentLiabilities" sheetId="6" r:id="rId6"/>
     <sheet name="Equity" sheetId="7" r:id="rId7"/>
+    <sheet name="NOTES_TradeReceivables" sheetId="8" r:id="rId8"/>
+    <sheet name="NOTES_NonCurrentLiabilities" sheetId="9" r:id="rId9"/>
+    <sheet name="NOTES_PlantEquipment" sheetId="10" r:id="rId10"/>
+    <sheet name="NOTES_IntangibleAssets" sheetId="13" r:id="rId11"/>
+    <sheet name="NOTES_Income" sheetId="14" r:id="rId12"/>
+    <sheet name="NOTES_Expenses" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>Note</t>
   </si>
@@ -101,13 +107,136 @@
     <t>Trade and Other Payables</t>
   </si>
   <si>
-    <t>Provision for Income Tax</t>
-  </si>
-  <si>
     <t>Issued Capital</t>
   </si>
   <si>
     <t>Reserves</t>
+  </si>
+  <si>
+    <t>Cash on hand</t>
+  </si>
+  <si>
+    <t>Trade Debtors</t>
+  </si>
+  <si>
+    <t>GST on Acquisitions</t>
+  </si>
+  <si>
+    <t>GST on Supplies</t>
+  </si>
+  <si>
+    <t>NOTES_TRADERECEIVABLES</t>
+  </si>
+  <si>
+    <t>NOTES_NonCurrentLiabilities</t>
+  </si>
+  <si>
+    <t>NOTES_PlantEquipment</t>
+  </si>
+  <si>
+    <t>NOTES_IntangibleAssets</t>
+  </si>
+  <si>
+    <t>Loans to Director Habib Zaiter</t>
+  </si>
+  <si>
+    <t>Loans to Related Companies</t>
+  </si>
+  <si>
+    <t>Plant &amp; Equipment - at cost</t>
+  </si>
+  <si>
+    <t>Less Prov'n for Depreciation</t>
+  </si>
+  <si>
+    <t>Motor Vehicles - at cost</t>
+  </si>
+  <si>
+    <t>Formation Expenses - at cost</t>
+  </si>
+  <si>
+    <t>NOTES_Expenses</t>
+  </si>
+  <si>
+    <t>NOTES_Income</t>
+  </si>
+  <si>
+    <t>Construction Services Revenue</t>
+  </si>
+  <si>
+    <t>Other Income - Job Keeper Payments</t>
+  </si>
+  <si>
+    <t>Employee Contribution MV Fringe Benefits</t>
+  </si>
+  <si>
+    <t>Accountancy</t>
+  </si>
+  <si>
+    <t>Advertising &amp; Promotion</t>
+  </si>
+  <si>
+    <t>Bank Charges</t>
+  </si>
+  <si>
+    <t>Cleaning</t>
+  </si>
+  <si>
+    <t>Consultants Fees</t>
+  </si>
+  <si>
+    <t>Computer Consumables</t>
+  </si>
+  <si>
+    <t>Depreciation and New Asset Write off</t>
+  </si>
+  <si>
+    <t>Donations</t>
+  </si>
+  <si>
+    <t>Electricity &amp; Gas</t>
+  </si>
+  <si>
+    <t>Filing Fees</t>
+  </si>
+  <si>
+    <t>Fines</t>
+  </si>
+  <si>
+    <t>Hire of Plant</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>Materials / Projects Costs</t>
+  </si>
+  <si>
+    <t>Motor Vehicle Expenses</t>
+  </si>
+  <si>
+    <t>Printing &amp; Stationery</t>
+  </si>
+  <si>
+    <t>Protective Clothing</t>
+  </si>
+  <si>
+    <t>Repairs &amp; Maintenance</t>
+  </si>
+  <si>
+    <t>Director Fee - Habib Zaiter</t>
+  </si>
+  <si>
+    <t>Staff Amenities</t>
+  </si>
+  <si>
+    <t>Telephone &amp; Internet</t>
+  </si>
+  <si>
+    <t>Travel &amp; Accommodation</t>
+  </si>
+  <si>
+    <t>Licenses Registrations &amp; Permits</t>
   </si>
 </sst>
 </file>
@@ -117,7 +246,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -131,6 +260,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,11 +289,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -516,6 +652,478 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F1E540-F171-FD41-A1CA-3222689178CB}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3">
+        <v>135000</v>
+      </c>
+      <c r="D2" s="3">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-21000</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-7500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="3">
+        <v>86467</v>
+      </c>
+      <c r="D4" s="3">
+        <v>86467</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-50580</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-35200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A215D4C0-9C99-AA40-8AC5-4AE1D307E90A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1600</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6FC1D7-1B9E-564C-9D8B-620C2D6DFC4D}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="3">
+        <v>484500</v>
+      </c>
+      <c r="D2" s="3">
+        <v>536727</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="3">
+        <v>21900</v>
+      </c>
+      <c r="D3" s="3">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4976</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3038</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B251F20E-19B8-C44E-8E23-B5F3BA38F7BE}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" style="4"/>
+    <col min="4" max="4" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="4">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="4">
+        <v>3250</v>
+      </c>
+      <c r="D2" s="4">
+        <v>4613</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1358</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4">
+        <v>133</v>
+      </c>
+      <c r="D4" s="4">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4">
+        <v>723</v>
+      </c>
+      <c r="D6" s="4">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="4">
+        <v>826</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="4">
+        <v>28880</v>
+      </c>
+      <c r="D8" s="4">
+        <v>21750</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="4">
+        <v>909</v>
+      </c>
+      <c r="D9" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="4">
+        <v>607</v>
+      </c>
+      <c r="D11" s="4">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="4">
+        <v>897</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="4">
+        <v>8295</v>
+      </c>
+      <c r="D14" s="4">
+        <v>8300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="4">
+        <v>544</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="4">
+        <v>7210</v>
+      </c>
+      <c r="D16" s="4">
+        <v>26018</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="4">
+        <v>17063</v>
+      </c>
+      <c r="D17" s="4">
+        <v>14784</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="4">
+        <v>140</v>
+      </c>
+      <c r="D18" s="4">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="4">
+        <v>282</v>
+      </c>
+      <c r="D19" s="4">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="4">
+        <v>356</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="4">
+        <v>25576</v>
+      </c>
+      <c r="D21" s="4">
+        <v>39645</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="4">
+        <v>479</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="4">
+        <v>6357</v>
+      </c>
+      <c r="D23" s="4">
+        <v>5298</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1653</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1332</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC16966-3B3C-254F-BB2D-E9831DF66171}">
   <dimension ref="A1:I9"/>
@@ -612,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{166F594D-BC78-8144-A8D3-8BB1AF0D82A8}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,10 +1248,22 @@
       <c r="A2" t="s">
         <v>15</v>
       </c>
+      <c r="C2" s="3">
+        <v>26344</v>
+      </c>
+      <c r="D2" s="3">
+        <v>27341</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
+      </c>
+      <c r="C3" s="3">
+        <v>577474</v>
+      </c>
+      <c r="D3" s="3">
+        <v>277801</v>
       </c>
     </row>
   </sheetData>
@@ -653,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34660CA8-F6EE-354F-A09C-EB1BD7F745BA}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,10 +1303,36 @@
       <c r="A2" t="s">
         <v>16</v>
       </c>
+      <c r="C2" s="3">
+        <v>149887</v>
+      </c>
+      <c r="D2" s="3">
+        <v>171967</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1600</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>
@@ -696,10 +1342,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C3FB75A-DFF3-CB45-A965-E4F722630F8D}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -725,10 +1371,11 @@
       <c r="A2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>19</v>
+      <c r="C2">
+        <v>37794</v>
+      </c>
+      <c r="D2">
+        <v>15194</v>
       </c>
     </row>
   </sheetData>
@@ -741,7 +1388,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -777,7 +1424,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -801,18 +1448,148 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5D57D7-5D01-3249-A202-03400A1239A5}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3">
+        <v>464564</v>
+      </c>
+      <c r="D2" s="3">
+        <v>227801</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C02C969F-2409-3245-A899-4C8B0C84D297}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>